<commit_message>
Add graph, Update data, README.md
</commit_message>
<xml_diff>
--- a/jun_kazama_data/jun-kazama-tekken-8-frame-data.xlsx
+++ b/jun_kazama_data/jun-kazama-tekken-8-frame-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DA\Tekken 8 Data Analysis\jun_kazama_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C98FED2-6ECB-44C3-8D1F-4FC01FDC1FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88B943D-E61B-4166-95EC-A300FE5DF9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="212">
   <si>
     <t>Command</t>
   </si>
@@ -587,79 +587,91 @@
     <t>Moves While Crouching</t>
   </si>
   <si>
+    <t>Heat Moves</t>
+  </si>
+  <si>
+    <t>Normal Moves</t>
+  </si>
+  <si>
+    <t>H,M,H</t>
+  </si>
+  <si>
+    <t>Rage Art</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1+4 </t>
+  </si>
+  <si>
+    <t>Moves During Genjitsu</t>
+  </si>
+  <si>
+    <t>Moves during Sidestep</t>
+  </si>
+  <si>
+    <t>Moves during Miare</t>
+  </si>
+  <si>
+    <t>Moves during Izumo</t>
+  </si>
+  <si>
+    <t>Moves during White Heron Dance</t>
+  </si>
+  <si>
+    <t>Launch Moves</t>
+  </si>
+  <si>
+    <t>H,L,M</t>
+  </si>
+  <si>
+    <t>Moves during Saika</t>
+  </si>
+  <si>
+    <t>M,H,M</t>
+  </si>
+  <si>
+    <t>M,H,H</t>
+  </si>
+  <si>
+    <t>H,Throw</t>
+  </si>
+  <si>
+    <t>L,H,H,M</t>
+  </si>
+  <si>
+    <t>L,H,H,L</t>
+  </si>
+  <si>
+    <t>L,H,M,M</t>
+  </si>
+  <si>
+    <t>L,H,H</t>
+  </si>
+  <si>
+    <t>L,H,M</t>
+  </si>
+  <si>
+    <t>L,H,M,L</t>
+  </si>
+  <si>
+    <t>Moves during Leg Cutter</t>
+  </si>
+  <si>
+    <t>Power Crush</t>
+  </si>
+  <si>
+    <t>Leg cutter 4, 4</t>
+  </si>
+  <si>
+    <t>L,L,L</t>
+  </si>
+  <si>
+    <t>L,sL,H</t>
+  </si>
+  <si>
     <t>Block(Only last action is considered or if the move is stopped when blocked)</t>
   </si>
   <si>
-    <t>Heat Moves</t>
-  </si>
-  <si>
-    <t>Normal Moves</t>
-  </si>
-  <si>
-    <t>H,M,H</t>
-  </si>
-  <si>
-    <t>Rage Art</t>
-  </si>
-  <si>
     <t>Hit(Only last action is considered)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1+4 </t>
-  </si>
-  <si>
-    <t>Moves During Genjitsu</t>
-  </si>
-  <si>
-    <t>Moves during Sidestep</t>
-  </si>
-  <si>
-    <t>Moves during Miare</t>
-  </si>
-  <si>
-    <t>Moves during Izumo</t>
-  </si>
-  <si>
-    <t>Moves during White Heron Dance</t>
-  </si>
-  <si>
-    <t>Launch Moves</t>
-  </si>
-  <si>
-    <t>H,L,M</t>
-  </si>
-  <si>
-    <t>Moves during Saika</t>
-  </si>
-  <si>
-    <t>M,H,M</t>
-  </si>
-  <si>
-    <t>M,H,H</t>
-  </si>
-  <si>
-    <t>H,Throw</t>
-  </si>
-  <si>
-    <t>L,H,H,M</t>
-  </si>
-  <si>
-    <t>L,H,H,L</t>
-  </si>
-  <si>
-    <t>L,H,M,M</t>
-  </si>
-  <si>
-    <t>L,H,H</t>
-  </si>
-  <si>
-    <t>L,H,M</t>
-  </si>
-  <si>
-    <t>L,H,M,L</t>
-  </si>
-  <si>
-    <t>Moves during Leg Cutter</t>
   </si>
 </sst>
 </file>
@@ -1040,25 +1052,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H149"/>
+  <dimension ref="A1:G150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="1.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1072,16 +1084,16 @@
         <v>180</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1101,13 +1113,10 @@
         <v>8</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1127,10 +1136,10 @@
         <v>8</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1150,13 +1159,10 @@
         <v>6</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1177,10 +1183,10 @@
         <v>11</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1200,10 +1206,10 @@
         <v>5</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1223,13 +1229,10 @@
         <v>10</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1249,10 +1252,10 @@
         <v>2</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1272,10 +1275,10 @@
         <v>7</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1296,10 +1299,10 @@
         <v>7</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -1320,10 +1323,10 @@
         <v>-1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1344,10 +1347,10 @@
         <v>10</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1368,10 +1371,10 @@
         <v>13</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1392,10 +1395,10 @@
         <v>48</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -1415,10 +1418,10 @@
         <v>18</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -1438,10 +1441,10 @@
         <v>7</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -1461,13 +1464,10 @@
         <v>17</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
@@ -1488,12 +1488,12 @@
         <v>26</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>33</v>
@@ -1512,10 +1512,10 @@
         <v>-3</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>34</v>
       </c>
@@ -1535,10 +1535,10 @@
         <v>9</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>35</v>
       </c>
@@ -1558,10 +1558,10 @@
         <v>33</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>36</v>
       </c>
@@ -1581,13 +1581,10 @@
         <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="H22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>37</v>
       </c>
@@ -1607,10 +1604,10 @@
         <v>7</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>38</v>
       </c>
@@ -1630,10 +1627,10 @@
         <v>11</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>40</v>
       </c>
@@ -1653,13 +1650,10 @@
         <v>14</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>41</v>
       </c>
@@ -1680,10 +1674,10 @@
         <v>28</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>42</v>
       </c>
@@ -1703,10 +1697,10 @@
         <v>13</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>43</v>
       </c>
@@ -1726,10 +1720,10 @@
         <v>26</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>44</v>
       </c>
@@ -1749,10 +1743,10 @@
         <v>0</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>45</v>
       </c>
@@ -1772,10 +1766,10 @@
         <v>25</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>46</v>
       </c>
@@ -1795,10 +1789,10 @@
         <v>8</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>47</v>
       </c>
@@ -1818,7 +1812,7 @@
         <v>2</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1841,7 +1835,7 @@
         <v>6</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1864,7 +1858,7 @@
         <v>29</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1887,7 +1881,7 @@
         <v>38</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1910,7 +1904,7 @@
         <v>19</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1933,7 +1927,7 @@
         <v>48</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1956,7 +1950,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1979,7 +1973,7 @@
         <v>17</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2002,7 +1996,7 @@
         <v>4</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2025,7 +2019,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2048,7 +2042,7 @@
         <v>-1</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2071,7 +2065,7 @@
         <v>13</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2094,7 +2088,7 @@
         <v>72</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2117,7 +2111,7 @@
         <v>30</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2140,7 +2134,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2164,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2188,67 +2182,76 @@
         <v>21</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="3">
         <v>15</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="3">
         <v>23</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="3">
+        <v>-12</v>
+      </c>
+      <c r="F49" s="3">
+        <v>2</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="3">
+        <v>14</v>
+      </c>
+      <c r="D50" s="3">
+        <v>18</v>
+      </c>
+      <c r="E50" s="3">
+        <v>-12</v>
+      </c>
+      <c r="F50" s="3">
+        <v>2</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="3">
+        <v>14</v>
+      </c>
+      <c r="D51" s="3">
+        <v>22</v>
+      </c>
+      <c r="E51" s="3">
         <v>-11</v>
       </c>
-      <c r="F49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50">
-        <v>14</v>
-      </c>
-      <c r="D50">
-        <v>18</v>
-      </c>
-      <c r="E50">
-        <v>-12</v>
-      </c>
-      <c r="F50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>71</v>
-      </c>
-      <c r="B51" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51">
-        <v>14</v>
-      </c>
-      <c r="D51">
-        <v>22</v>
-      </c>
-      <c r="E51">
-        <v>-11</v>
-      </c>
-      <c r="F51">
-        <v>0</v>
+      <c r="F51" s="3">
+        <v>0</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2271,7 +2274,7 @@
         <v>6</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2294,70 +2297,76 @@
         <v>0</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B54" t="s">
-        <v>27</v>
-      </c>
-      <c r="C54">
+      <c r="B54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="3">
         <v>10</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="3">
         <v>14</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="3">
         <v>-9</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+      <c r="G54" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="3">
         <v>17</v>
       </c>
-      <c r="D55">
-        <v>14</v>
-      </c>
-      <c r="E55">
+      <c r="D55" s="3">
+        <v>15</v>
+      </c>
+      <c r="E55" s="3">
         <v>-9</v>
       </c>
-      <c r="F55">
-        <v>8</v>
-      </c>
-      <c r="G55" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="F55" s="3">
+        <v>2</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="3">
         <v>20</v>
       </c>
-      <c r="D56">
-        <v>14</v>
-      </c>
-      <c r="E56">
+      <c r="D56" s="3">
+        <v>16</v>
+      </c>
+      <c r="E56" s="3">
         <v>-9</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="3">
         <v>3</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="57" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2380,7 +2389,7 @@
         <v>22</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2403,7 +2412,7 @@
         <v>67</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="59" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -2426,47 +2435,53 @@
         <v>20</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B60" t="s">
-        <v>27</v>
-      </c>
-      <c r="C60">
+      <c r="B60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="3">
         <v>14</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="3">
         <v>13</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="3">
         <v>-7</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+      <c r="G60" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="3">
         <v>31</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="3">
         <v>13</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="3">
         <v>-13</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="3">
         <v>5</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2489,27 +2504,30 @@
         <v>0</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B63" t="s">
-        <v>27</v>
-      </c>
-      <c r="C63">
-        <v>21</v>
-      </c>
-      <c r="D63">
+      <c r="B63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="3">
+        <v>25</v>
+      </c>
+      <c r="D63" s="3">
         <v>28</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="3">
         <v>-12</v>
       </c>
-      <c r="F63">
-        <v>7</v>
+      <c r="F63" s="3">
+        <v>9</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2535,24 +2553,27 @@
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+    <row r="65" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="3">
         <v>17</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="3">
         <v>23</v>
       </c>
-      <c r="E65">
-        <v>-5</v>
-      </c>
-      <c r="F65">
-        <v>10</v>
+      <c r="E65" s="3">
+        <v>6</v>
+      </c>
+      <c r="F65" s="3">
+        <v>11</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="66" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2575,7 +2596,7 @@
         <v>22</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2598,7 +2619,7 @@
         <v>12</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2621,47 +2642,53 @@
         <v>30</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B69" t="s">
-        <v>27</v>
-      </c>
-      <c r="C69">
+      <c r="B69" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" s="3">
         <v>17</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="3">
         <v>20</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="3">
         <v>-6</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+      <c r="G69" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B70" t="s">
-        <v>27</v>
-      </c>
-      <c r="C70">
+      <c r="B70" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C70" s="3">
         <v>10</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="3">
         <v>16</v>
       </c>
-      <c r="E70">
-        <v>-19</v>
-      </c>
-      <c r="F70">
+      <c r="E70" s="3">
+        <v>-20</v>
+      </c>
+      <c r="F70" s="3">
         <v>-9</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="71" spans="1:7" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2685,7 +2712,7 @@
         <v>84</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2708,67 +2735,76 @@
         <v>18</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B73" t="s">
-        <v>27</v>
-      </c>
-      <c r="C73">
+      <c r="B73" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C73" s="3">
         <v>16</v>
       </c>
-      <c r="D73">
-        <v>18</v>
-      </c>
-      <c r="E73">
+      <c r="D73" s="3">
+        <v>16</v>
+      </c>
+      <c r="E73" s="3">
         <v>-12</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+      <c r="G73" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B74" t="s">
-        <v>27</v>
-      </c>
-      <c r="C74">
+      <c r="B74" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" s="3">
         <v>16</v>
       </c>
-      <c r="D74">
-        <v>18</v>
-      </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-      <c r="F74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+      <c r="D74" s="3">
+        <v>16</v>
+      </c>
+      <c r="E74" s="3">
+        <v>1</v>
+      </c>
+      <c r="F74" s="3">
+        <v>16</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B75" t="s">
-        <v>27</v>
-      </c>
-      <c r="C75">
+      <c r="B75" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75" s="3">
         <v>16</v>
       </c>
-      <c r="D75">
-        <v>18</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="F75">
-        <v>0</v>
+      <c r="D75" s="3">
+        <v>16</v>
+      </c>
+      <c r="E75" s="3">
+        <v>1</v>
+      </c>
+      <c r="F75" s="3">
+        <v>16</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2791,7 +2827,7 @@
         <v>8</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="77" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2814,7 +2850,7 @@
         <v>29</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="78" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2837,7 +2873,7 @@
         <v>2</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="79" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -2860,7 +2896,7 @@
         <v>14</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="80" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2883,7 +2919,7 @@
         <v>23</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="81" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2906,87 +2942,99 @@
         <v>14</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="3">
         <v>14</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="3">
         <v>12</v>
       </c>
-      <c r="E82">
+      <c r="E82" s="3">
         <v>-6</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+      <c r="G82" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="3">
         <v>21</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="3">
         <v>12</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="3">
         <v>-9</v>
       </c>
-      <c r="F83">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+      <c r="F83" s="3">
+        <v>2</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="3">
         <v>30</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="3">
         <v>12</v>
       </c>
-      <c r="E84">
-        <v>-10</v>
-      </c>
-      <c r="F84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+      <c r="E84" s="3">
+        <v>-11</v>
+      </c>
+      <c r="F84" s="3">
+        <v>0</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="3">
         <v>47</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="3">
         <v>12</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="3">
         <v>-16</v>
       </c>
-      <c r="F85">
-        <v>0</v>
+      <c r="F85" s="3">
+        <v>0</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="86" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3012,24 +3060,27 @@
         <v>182</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="87" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B87" t="s">
-        <v>27</v>
-      </c>
-      <c r="C87">
+      <c r="B87" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C87" s="3">
         <v>12</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="3">
         <v>13</v>
       </c>
-      <c r="E87">
+      <c r="E87" s="3">
         <v>-8</v>
       </c>
-      <c r="F87">
+      <c r="F87" s="3">
         <v>5</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3075,7 +3126,7 @@
         <v>25</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="90" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3101,24 +3152,27 @@
         <v>182</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    <row r="91" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B91" t="s">
-        <v>27</v>
-      </c>
-      <c r="C91">
+      <c r="B91" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C91" s="3">
         <v>20</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="3">
         <v>21</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="3">
         <v>-2</v>
       </c>
-      <c r="F91">
+      <c r="F91" s="3">
         <v>5</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="92" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -3144,24 +3198,27 @@
         <v>182</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+    <row r="93" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="3">
         <v>20</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="3">
         <v>21</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="3">
         <v>-6</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="3">
         <v>5</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="94" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -3184,7 +3241,7 @@
         <v>15</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="95" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3207,44 +3264,53 @@
         <v>26</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="3">
         <v>12</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="3">
         <v>16</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="3">
         <v>-11</v>
       </c>
-      <c r="F96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+      <c r="F96" s="3">
+        <v>0</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="3">
         <v>15</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="3">
         <v>21</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="3">
         <v>-19</v>
+      </c>
+      <c r="F97" s="3">
+        <v>10</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="98" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3267,7 +3333,7 @@
         <v>14</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="99" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -3290,47 +3356,53 @@
         <v>17</v>
       </c>
       <c r="G99" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" s="3">
+        <v>34</v>
+      </c>
+      <c r="D100" s="3">
+        <v>16</v>
+      </c>
+      <c r="E100" s="3">
+        <v>-4</v>
+      </c>
+      <c r="F100" s="3">
+        <v>7</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" s="3">
+        <v>24</v>
+      </c>
+      <c r="D101" s="3">
+        <v>23</v>
+      </c>
+      <c r="E101" s="3">
+        <v>-7</v>
+      </c>
+      <c r="F101" s="3">
+        <v>4</v>
+      </c>
+      <c r="G101" s="3" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
-        <v>126</v>
-      </c>
-      <c r="B100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C100">
-        <v>34</v>
-      </c>
-      <c r="D100">
-        <v>16</v>
-      </c>
-      <c r="E100">
-        <v>-4</v>
-      </c>
-      <c r="F100">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>127</v>
-      </c>
-      <c r="B101" t="s">
-        <v>4</v>
-      </c>
-      <c r="C101">
-        <v>7</v>
-      </c>
-      <c r="D101">
-        <v>12</v>
-      </c>
-      <c r="E101">
-        <v>-7</v>
-      </c>
-      <c r="F101">
-        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3353,7 +3425,7 @@
         <v>30</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="103" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3377,7 +3449,7 @@
         <v>6</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="104" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3400,7 +3472,7 @@
         <v>34</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="105" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3408,7 +3480,7 @@
         <v>131</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C105" s="3">
         <f>17+10+16</f>
@@ -3424,27 +3496,31 @@
         <v>17</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B106" t="s">
-        <v>59</v>
-      </c>
-      <c r="C106">
-        <v>15</v>
-      </c>
-      <c r="D106">
-        <v>20</v>
-      </c>
-      <c r="E106">
+      <c r="B106" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C106" s="3">
+        <f>17+15</f>
+        <v>32</v>
+      </c>
+      <c r="D106" s="3">
+        <v>23</v>
+      </c>
+      <c r="E106" s="3">
         <v>-37</v>
       </c>
-      <c r="F106">
+      <c r="F106" s="3">
         <v>-1</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="107" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3452,7 +3528,7 @@
         <v>133</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C107" s="3">
         <f>17+36</f>
@@ -3468,107 +3544,124 @@
         <v>15</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B108" t="s">
-        <v>27</v>
-      </c>
-      <c r="C108">
-        <v>24</v>
-      </c>
-      <c r="D108">
+      <c r="B108" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108" s="3">
+        <f>24+17</f>
+        <v>41</v>
+      </c>
+      <c r="D108" s="3">
+        <v>23</v>
+      </c>
+      <c r="E108" s="3">
+        <v>-12</v>
+      </c>
+      <c r="F108" s="3">
+        <v>19</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109" s="3">
+        <f>21+17</f>
+        <v>38</v>
+      </c>
+      <c r="D109" s="3">
+        <v>23</v>
+      </c>
+      <c r="E109" s="3">
+        <v>-9</v>
+      </c>
+      <c r="F109" s="3">
+        <v>2</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C110" s="3">
+        <v>22</v>
+      </c>
+      <c r="D110" s="3">
         <v>20</v>
       </c>
-      <c r="E108">
-        <v>-12</v>
-      </c>
-      <c r="F108">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
-        <v>136</v>
-      </c>
-      <c r="B109" t="s">
-        <v>27</v>
-      </c>
-      <c r="C109">
-        <v>21</v>
-      </c>
-      <c r="D109">
-        <v>15</v>
-      </c>
-      <c r="E109">
-        <v>-9</v>
-      </c>
-      <c r="F109">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
-        <v>137</v>
-      </c>
-      <c r="B110" t="s">
-        <v>59</v>
-      </c>
-      <c r="C110">
-        <v>22</v>
-      </c>
-      <c r="D110">
-        <v>19</v>
-      </c>
-      <c r="E110">
+      <c r="E110" s="3">
         <v>-13</v>
       </c>
-      <c r="F110">
+      <c r="F110" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+      <c r="G110" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B111" t="s">
-        <v>27</v>
-      </c>
-      <c r="C111">
+      <c r="B111" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C111" s="3">
         <v>48</v>
       </c>
-      <c r="D111">
-        <v>15</v>
-      </c>
-      <c r="E111">
+      <c r="D111" s="3">
+        <v>16</v>
+      </c>
+      <c r="E111" s="3">
         <v>-13</v>
       </c>
-      <c r="F111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
+      <c r="F111" s="3">
+        <v>0</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B112" t="s">
-        <v>27</v>
-      </c>
-      <c r="C112">
+      <c r="B112" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C112" s="3">
         <v>14</v>
       </c>
-      <c r="D112">
-        <v>16</v>
-      </c>
-      <c r="E112">
+      <c r="D112" s="3">
+        <v>17</v>
+      </c>
+      <c r="E112" s="3">
         <v>-4</v>
       </c>
-      <c r="F112">
+      <c r="F112" s="3">
         <v>4</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="113" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -3591,7 +3684,7 @@
         <v>33</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="114" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3614,7 +3707,7 @@
         <v>26</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="115" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3637,7 +3730,7 @@
         <v>72</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="116" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -3660,27 +3753,30 @@
         <v>17</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C117">
+      <c r="C117" s="3">
         <v>17</v>
       </c>
-      <c r="D117">
-        <v>22</v>
-      </c>
-      <c r="E117">
-        <v>-5</v>
-      </c>
-      <c r="F117">
-        <v>10</v>
+      <c r="D117" s="3">
+        <v>23</v>
+      </c>
+      <c r="E117" s="3">
+        <v>6</v>
+      </c>
+      <c r="F117" s="3">
+        <v>11</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="118" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3703,7 +3799,7 @@
         <v>0</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="119" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3726,47 +3822,55 @@
         <v>0</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B120" t="s">
-        <v>59</v>
-      </c>
-      <c r="C120">
-        <v>15</v>
-      </c>
-      <c r="D120">
-        <v>0</v>
-      </c>
-      <c r="E120">
-        <v>-11</v>
-      </c>
-      <c r="F120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+      <c r="B120" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C120" s="3">
+        <f>14+15</f>
+        <v>29</v>
+      </c>
+      <c r="D120" s="3">
+        <v>22</v>
+      </c>
+      <c r="E120" s="3">
+        <v>-7</v>
+      </c>
+      <c r="F120" s="3">
+        <v>4</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B121" t="s">
-        <v>33</v>
-      </c>
-      <c r="C121">
-        <v>13</v>
-      </c>
-      <c r="D121">
-        <v>0</v>
-      </c>
-      <c r="E121">
+      <c r="B121" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C121" s="3">
+        <f>13+14</f>
+        <v>27</v>
+      </c>
+      <c r="D121" s="3">
+        <v>22</v>
+      </c>
+      <c r="E121" s="3">
         <v>-3</v>
       </c>
-      <c r="F121">
-        <v>0</v>
+      <c r="F121" s="3">
+        <v>-3</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="122" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3774,7 +3878,7 @@
         <v>150</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C122" s="3">
         <f>8+5+10</f>
@@ -3790,7 +3894,7 @@
         <v>9</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="123" spans="1:7" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3798,7 +3902,7 @@
         <v>151</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C123" s="3">
         <f>5+8+10+23</f>
@@ -3814,7 +3918,7 @@
         <v>11</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="124" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3822,7 +3926,7 @@
         <v>152</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C124" s="3">
         <f>5+8+10+15</f>
@@ -3838,7 +3942,7 @@
         <v>27</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="125" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3846,7 +3950,7 @@
         <v>153</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C125" s="3">
         <f>8+5+15</f>
@@ -3862,7 +3966,7 @@
         <v>1</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="126" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3870,7 +3974,7 @@
         <v>154</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C126" s="3">
         <f>5+8+15+20</f>
@@ -3886,7 +3990,7 @@
         <v>17</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="127" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3894,7 +3998,7 @@
         <v>155</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C127" s="3">
         <v>32</v>
@@ -3909,7 +4013,7 @@
         <v>4</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="128" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3917,7 +4021,7 @@
         <v>156</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C128" s="3">
         <v>37</v>
@@ -3932,15 +4036,15 @@
         <v>13</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C129" s="3">
         <f>22+17</f>
@@ -3956,15 +4060,15 @@
         <v>30</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
         <v>158</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C130" s="3">
         <f>24+17</f>
@@ -3980,10 +4084,10 @@
         <v>42</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>159</v>
       </c>
@@ -4003,10 +4107,10 @@
         <v>0</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
         <v>160</v>
       </c>
@@ -4026,10 +4130,10 @@
         <v>0</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
         <v>161</v>
       </c>
@@ -4052,7 +4156,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="134" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
         <v>163</v>
       </c>
@@ -4075,7 +4179,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="135" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>164</v>
       </c>
@@ -4098,7 +4202,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="136" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>165</v>
       </c>
@@ -4121,7 +4225,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="137" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
         <v>166</v>
       </c>
@@ -4144,12 +4248,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="138" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C138" s="3">
         <f>35+17</f>
@@ -4168,7 +4272,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="139" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
         <v>168</v>
       </c>
@@ -4188,13 +4292,10 @@
         <v>2</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="H139" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
         <v>169</v>
       </c>
@@ -4214,10 +4315,10 @@
         <v>21</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
         <v>170</v>
       </c>
@@ -4238,10 +4339,10 @@
         <v>23</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>171</v>
       </c>
@@ -4261,10 +4362,10 @@
         <v>26</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="s">
         <v>172</v>
       </c>
@@ -4284,10 +4385,10 @@
         <v>43</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
         <v>173</v>
       </c>
@@ -4308,10 +4409,10 @@
         <v>42</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A145" s="3" t="s">
         <v>174</v>
       </c>
@@ -4331,15 +4432,15 @@
         <v>67</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="s">
         <v>175</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C146" s="3">
         <f>18+11+17</f>
@@ -4355,10 +4456,10 @@
         <v>36</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
         <v>176</v>
       </c>
@@ -4378,10 +4479,10 @@
         <v>36</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A148" s="3" t="s">
         <v>177</v>
       </c>
@@ -4402,10 +4503,10 @@
         <v>0</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A149" s="3" t="s">
         <v>178</v>
       </c>
@@ -4427,8 +4528,29 @@
       <c r="G149" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="H149" s="3">
-        <v>0</v>
+    </row>
+    <row r="150" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C150" s="3">
+        <f>14+15+16</f>
+        <v>45</v>
+      </c>
+      <c r="D150" s="3">
+        <v>22</v>
+      </c>
+      <c r="E150" s="3">
+        <v>-7</v>
+      </c>
+      <c r="F150" s="3">
+        <v>4</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>